<commit_message>
completed locations on the final file
still missing the code of the maps and we still need ecosystems
</commit_message>
<xml_diff>
--- a/SquareMileage.xlsx
+++ b/SquareMileage.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11108"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/veronicamarquez/Desktop/Dr.D Ecology Bias SC/MA321-Daneshgar/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/odalysbar/Documents/monmouthuni/MA321-FA20/MA321-Daneshgar/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{53D5D62A-D34A-494A-A753-4EF49B30539C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10020" yWindow="460" windowWidth="18780" windowHeight="16520" tabRatio="500"/>
+    <workbookView xWindow="14520" yWindow="0" windowWidth="14280" windowHeight="18000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="86">
   <si>
     <t>Continent</t>
   </si>
@@ -282,12 +283,15 @@
   </si>
   <si>
     <t>Sq.mi (mi^2)</t>
+  </si>
+  <si>
+    <t>stateSQM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -335,8 +339,23 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{07090D75-9D27-864A-B066-E5065AF1E24A}" name="Table1" displayName="Table1" ref="D1:F51" totalsRowShown="0">
+  <autoFilter ref="D1:F51" xr:uid="{F72EF95D-EC68-C742-80CD-2F052C045650}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{E474624B-F098-7749-8DDD-83082DC986CB}" name="U.S. States"/>
+    <tableColumn id="3" xr3:uid="{DC7360F2-B0CA-F94C-937C-5C3A6028F94A}" name="stateSQM"/>
+    <tableColumn id="2" xr3:uid="{58FF40DC-05A5-CB44-B04E-A34E6EBCBDF5}" name="Total Sq. mi (mi^2)"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -601,51 +620,58 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:J52"/>
+  <dimension ref="A1:L52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="140" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="140" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="11.6640625" customWidth="1"/>
+    <col min="5" max="5" width="18.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>10</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>12</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>13</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>24</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>79</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -655,29 +681,35 @@
       <c r="C2" t="s">
         <v>28</v>
       </c>
-      <c r="D2">
+      <c r="D2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2">
+        <v>656424</v>
+      </c>
+      <c r="F2">
         <v>52423</v>
       </c>
-      <c r="E2">
+      <c r="G2">
         <v>50750</v>
       </c>
-      <c r="F2">
+      <c r="H2">
         <v>1673</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>14</v>
       </c>
-      <c r="H2">
+      <c r="J2">
         <v>191308</v>
       </c>
-      <c r="I2" t="s">
+      <c r="K2" t="s">
         <v>80</v>
       </c>
-      <c r="J2">
+      <c r="L2">
         <v>161913</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -687,29 +719,35 @@
       <c r="C3" t="s">
         <v>29</v>
       </c>
-      <c r="D3">
+      <c r="D3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3">
+        <v>52423</v>
+      </c>
+      <c r="F3">
         <v>656424</v>
       </c>
-      <c r="E3">
+      <c r="G3">
         <v>570374</v>
       </c>
-      <c r="F3">
+      <c r="H3">
         <v>86051</v>
       </c>
-      <c r="G3" t="s">
+      <c r="I3" t="s">
         <v>15</v>
       </c>
-      <c r="H3">
+      <c r="J3">
         <v>292589</v>
       </c>
-      <c r="I3" t="s">
+      <c r="K3" t="s">
         <v>81</v>
       </c>
-      <c r="J3">
+      <c r="L3">
         <v>750576</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -719,29 +757,35 @@
       <c r="C4" t="s">
         <v>30</v>
       </c>
-      <c r="D4">
+      <c r="D4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4">
         <v>114006</v>
       </c>
-      <c r="E4">
+      <c r="F4">
+        <v>114006</v>
+      </c>
+      <c r="G4">
         <v>113642</v>
       </c>
-      <c r="F4">
+      <c r="H4">
         <v>364</v>
       </c>
-      <c r="G4" t="s">
+      <c r="I4" t="s">
         <v>16</v>
       </c>
-      <c r="H4">
+      <c r="J4">
         <v>299170</v>
       </c>
-      <c r="I4" t="s">
+      <c r="K4" t="s">
         <v>82</v>
       </c>
-      <c r="J4">
+      <c r="L4">
         <v>919331</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -751,29 +795,35 @@
       <c r="C5" t="s">
         <v>31</v>
       </c>
-      <c r="D5">
+      <c r="D5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5">
+        <v>163707</v>
+      </c>
+      <c r="F5">
         <v>53182</v>
       </c>
-      <c r="E5">
+      <c r="G5">
         <v>52075</v>
       </c>
-      <c r="F5">
+      <c r="H5">
         <v>1107</v>
       </c>
-      <c r="G5" t="s">
+      <c r="I5" t="s">
         <v>17</v>
       </c>
-      <c r="H5">
+      <c r="J5">
         <v>5469</v>
       </c>
-      <c r="I5" t="s">
+      <c r="K5" t="s">
         <v>83</v>
       </c>
-      <c r="J5">
+      <c r="L5">
         <v>1873251</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -783,23 +833,29 @@
       <c r="C6" t="s">
         <v>32</v>
       </c>
-      <c r="D6">
+      <c r="D6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6">
+        <v>104100</v>
+      </c>
+      <c r="F6">
         <v>163707</v>
       </c>
-      <c r="E6">
+      <c r="G6">
         <v>155973</v>
       </c>
-      <c r="F6">
+      <c r="H6">
         <v>7734</v>
       </c>
-      <c r="G6" t="s">
+      <c r="I6" t="s">
         <v>18</v>
       </c>
-      <c r="H6" t="s">
+      <c r="J6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -809,23 +865,29 @@
       <c r="C7" t="s">
         <v>33</v>
       </c>
-      <c r="D7">
+      <c r="D7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7">
+        <v>59988</v>
+      </c>
+      <c r="F7">
         <v>104100</v>
       </c>
-      <c r="E7">
+      <c r="G7">
         <v>103730</v>
       </c>
-      <c r="F7">
+      <c r="H7">
         <v>371</v>
       </c>
-      <c r="G7" t="s">
+      <c r="I7" t="s">
         <v>19</v>
       </c>
-      <c r="H7">
+      <c r="J7">
         <v>444100</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -835,659 +897,926 @@
       <c r="C8" t="s">
         <v>34</v>
       </c>
-      <c r="D8">
+      <c r="D8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8">
+        <v>6459</v>
+      </c>
+      <c r="F8">
         <v>5544</v>
       </c>
-      <c r="E8">
+      <c r="G8">
         <v>4845</v>
       </c>
-      <c r="F8">
+      <c r="H8">
         <v>698</v>
       </c>
-      <c r="G8" t="s">
+      <c r="I8" t="s">
         <v>20</v>
       </c>
-      <c r="H8" t="s">
+      <c r="J8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
         <v>35</v>
       </c>
-      <c r="D9">
+      <c r="D9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9">
+        <v>36420</v>
+      </c>
+      <c r="F9">
         <v>2489</v>
       </c>
-      <c r="E9">
+      <c r="G9">
         <v>1955</v>
       </c>
-      <c r="F9">
+      <c r="H9">
         <v>535</v>
       </c>
-      <c r="G9" t="s">
+      <c r="I9" t="s">
         <v>21</v>
       </c>
-      <c r="H9">
+      <c r="J9">
         <v>507900</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
         <v>36</v>
       </c>
-      <c r="D10">
+      <c r="D10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10">
+        <v>82282</v>
+      </c>
+      <c r="F10">
         <v>59988</v>
       </c>
-      <c r="E10">
+      <c r="G10">
         <v>53997</v>
       </c>
-      <c r="F10">
+      <c r="H10">
         <v>5991</v>
       </c>
-      <c r="G10" t="s">
+      <c r="I10" t="s">
         <v>22</v>
       </c>
-      <c r="H10">
+      <c r="J10">
         <v>71992</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C11" t="s">
         <v>37</v>
       </c>
-      <c r="D11">
+      <c r="D11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11">
+        <v>10555</v>
+      </c>
+      <c r="F11">
         <v>59441</v>
       </c>
-      <c r="E11">
+      <c r="G11">
         <v>57919</v>
       </c>
-      <c r="F11">
+      <c r="H11">
         <v>1522</v>
       </c>
-      <c r="G11" t="s">
+      <c r="I11" t="s">
         <v>23</v>
       </c>
-      <c r="H11" t="s">
+      <c r="J11" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C12" t="s">
         <v>38</v>
       </c>
-      <c r="D12">
+      <c r="D12" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12">
+        <v>12407</v>
+      </c>
+      <c r="F12">
         <v>6459</v>
       </c>
-      <c r="E12">
+      <c r="G12">
         <v>6423</v>
       </c>
-      <c r="F12">
+      <c r="H12">
         <v>36</v>
       </c>
-      <c r="G12" t="s">
+      <c r="I12" t="s">
         <v>26</v>
       </c>
-      <c r="H12" t="s">
+      <c r="J12" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C13" t="s">
         <v>39</v>
       </c>
-      <c r="D13">
+      <c r="D13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13">
+        <v>96810</v>
+      </c>
+      <c r="F13">
         <v>83574</v>
       </c>
-      <c r="E13">
+      <c r="G13">
         <v>82751</v>
       </c>
-      <c r="F13">
+      <c r="H13">
         <v>823</v>
       </c>
-      <c r="G13" t="s">
+      <c r="I13" t="s">
         <v>27</v>
       </c>
-      <c r="H13" t="s">
+      <c r="J13" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C14" t="s">
         <v>40</v>
       </c>
-      <c r="D14">
+      <c r="D14" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14">
+        <v>69709</v>
+      </c>
+      <c r="F14">
         <v>57918</v>
       </c>
-      <c r="E14">
+      <c r="G14">
         <v>55593</v>
       </c>
-      <c r="F14">
+      <c r="H14">
         <v>2325</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C15" t="s">
         <v>41</v>
       </c>
-      <c r="D15">
+      <c r="D15" t="s">
+        <v>53</v>
+      </c>
+      <c r="E15">
+        <v>147046</v>
+      </c>
+      <c r="F15">
         <v>36420</v>
       </c>
-      <c r="E15">
+      <c r="G15">
         <v>35870</v>
       </c>
-      <c r="F15">
+      <c r="H15">
         <v>550</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C16" t="s">
         <v>42</v>
       </c>
-      <c r="D16">
+      <c r="D16" t="s">
+        <v>60</v>
+      </c>
+      <c r="E16">
+        <v>52672</v>
+      </c>
+      <c r="F16">
         <v>56276</v>
       </c>
-      <c r="E16">
+      <c r="G16">
         <v>55875</v>
       </c>
-      <c r="F16">
+      <c r="H16">
         <v>401</v>
       </c>
     </row>
-    <row r="17" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C17" t="s">
         <v>43</v>
       </c>
-      <c r="D17">
+      <c r="D17" t="s">
+        <v>56</v>
+      </c>
+      <c r="E17">
+        <v>9351</v>
+      </c>
+      <c r="F17">
         <v>82282</v>
       </c>
-      <c r="E17">
+      <c r="G17">
         <v>81823</v>
       </c>
-      <c r="F17">
+      <c r="H17">
         <v>459</v>
       </c>
     </row>
-    <row r="18" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C18" t="s">
         <v>44</v>
       </c>
-      <c r="D18">
+      <c r="D18" t="s">
+        <v>57</v>
+      </c>
+      <c r="E18">
+        <v>8722</v>
+      </c>
+      <c r="F18">
         <v>40411</v>
       </c>
-      <c r="E18">
+      <c r="G18">
         <v>39732</v>
       </c>
-      <c r="F18">
+      <c r="H18">
         <v>679</v>
       </c>
     </row>
-    <row r="19" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C19" t="s">
         <v>45</v>
       </c>
-      <c r="D19">
+      <c r="D19" t="s">
+        <v>58</v>
+      </c>
+      <c r="E19">
+        <v>121598</v>
+      </c>
+      <c r="F19">
         <v>51843</v>
       </c>
-      <c r="E19">
+      <c r="G19">
         <v>43566</v>
       </c>
-      <c r="F19">
+      <c r="H19">
         <v>8277</v>
       </c>
     </row>
-    <row r="20" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C20" t="s">
         <v>46</v>
       </c>
-      <c r="D20">
+      <c r="D20" t="s">
+        <v>59</v>
+      </c>
+      <c r="E20">
+        <v>54475</v>
+      </c>
+      <c r="F20">
         <v>35387</v>
       </c>
-      <c r="E20">
+      <c r="G20">
         <v>30865</v>
       </c>
-      <c r="F20">
+      <c r="H20">
         <v>4523</v>
       </c>
     </row>
-    <row r="21" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C21" t="s">
         <v>47</v>
       </c>
-      <c r="D21">
+      <c r="D21" t="s">
+        <v>62</v>
+      </c>
+      <c r="E21">
+        <v>44828</v>
+      </c>
+      <c r="F21">
         <v>12407</v>
       </c>
-      <c r="E21">
+      <c r="G21">
         <v>9775</v>
       </c>
-      <c r="F21">
+      <c r="H21">
         <v>2633</v>
       </c>
     </row>
-    <row r="22" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C22" t="s">
         <v>48</v>
       </c>
-      <c r="D22">
+      <c r="D22" t="s">
+        <v>64</v>
+      </c>
+      <c r="E22">
+        <v>98386</v>
+      </c>
+      <c r="F22">
         <v>10555</v>
       </c>
-      <c r="E22">
+      <c r="G22">
         <v>7838</v>
       </c>
-      <c r="F22">
+      <c r="H22">
         <v>2717</v>
       </c>
     </row>
-    <row r="23" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C23" t="s">
         <v>49</v>
       </c>
-      <c r="D23">
+      <c r="D23" t="s">
+        <v>70</v>
+      </c>
+      <c r="E23">
+        <v>268601</v>
+      </c>
+      <c r="F23">
         <v>96810</v>
       </c>
-      <c r="E23">
+      <c r="G23">
         <v>56809</v>
       </c>
-      <c r="F23">
+      <c r="H23">
         <v>40001</v>
       </c>
     </row>
-    <row r="24" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C24" t="s">
         <v>50</v>
       </c>
-      <c r="D24">
+      <c r="D24" t="s">
+        <v>71</v>
+      </c>
+      <c r="E24">
+        <v>84904</v>
+      </c>
+      <c r="F24">
         <v>86943</v>
       </c>
-      <c r="E24">
+      <c r="G24">
         <v>79617</v>
       </c>
-      <c r="F24">
+      <c r="H24">
         <v>7326</v>
       </c>
     </row>
-    <row r="25" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C25" t="s">
         <v>51</v>
       </c>
-      <c r="D25">
+      <c r="D25" t="s">
+        <v>74</v>
+      </c>
+      <c r="E25">
+        <v>71303</v>
+      </c>
+      <c r="F25">
         <v>48434</v>
       </c>
-      <c r="E25">
+      <c r="G25">
         <v>46914</v>
       </c>
-      <c r="F25">
+      <c r="H25">
         <v>1520</v>
       </c>
     </row>
-    <row r="26" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C26" t="s">
         <v>52</v>
       </c>
-      <c r="D26">
+      <c r="D26" t="s">
+        <v>76</v>
+      </c>
+      <c r="E26">
+        <v>65503</v>
+      </c>
+      <c r="F26">
         <v>69709</v>
       </c>
-      <c r="E26">
+      <c r="G26">
         <v>68898</v>
       </c>
-      <c r="F26">
+      <c r="H26">
         <v>811</v>
       </c>
     </row>
-    <row r="27" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C27" t="s">
         <v>53</v>
       </c>
-      <c r="D27">
+      <c r="D27" t="s">
+        <v>77</v>
+      </c>
+      <c r="E27">
+        <v>97818</v>
+      </c>
+      <c r="F27">
         <v>147046</v>
       </c>
-      <c r="E27">
+      <c r="G27">
         <v>145556</v>
       </c>
-      <c r="F27">
+      <c r="H27">
         <v>1490</v>
       </c>
     </row>
-    <row r="28" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C28" t="s">
         <v>54</v>
       </c>
-      <c r="D28">
+      <c r="D28" t="s">
+        <v>31</v>
+      </c>
+      <c r="E28">
+        <v>53182</v>
+      </c>
+      <c r="F28">
         <v>77358</v>
       </c>
-      <c r="E28">
+      <c r="G28">
         <v>76878</v>
       </c>
-      <c r="F28">
+      <c r="H28">
         <v>481</v>
       </c>
     </row>
-    <row r="29" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C29" t="s">
         <v>55</v>
       </c>
-      <c r="D29">
+      <c r="D29" t="s">
+        <v>34</v>
+      </c>
+      <c r="E29">
+        <v>5544</v>
+      </c>
+      <c r="F29">
         <v>110567</v>
       </c>
-      <c r="E29">
+      <c r="G29">
         <v>109806</v>
       </c>
-      <c r="F29">
+      <c r="H29">
         <v>761</v>
       </c>
     </row>
-    <row r="30" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C30" t="s">
         <v>56</v>
       </c>
-      <c r="D30">
+      <c r="D30" t="s">
+        <v>35</v>
+      </c>
+      <c r="E30">
+        <v>2489</v>
+      </c>
+      <c r="F30">
         <v>9351</v>
       </c>
-      <c r="E30">
+      <c r="G30">
         <v>8969</v>
       </c>
-      <c r="F30">
+      <c r="H30">
         <v>382</v>
       </c>
     </row>
-    <row r="31" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C31" t="s">
         <v>57</v>
       </c>
-      <c r="D31">
+      <c r="D31" t="s">
+        <v>37</v>
+      </c>
+      <c r="E31">
+        <v>59441</v>
+      </c>
+      <c r="F31">
         <v>8722</v>
       </c>
-      <c r="E31">
+      <c r="G31">
         <v>7419</v>
       </c>
-      <c r="F31">
+      <c r="H31">
         <v>1303</v>
       </c>
     </row>
-    <row r="32" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C32" t="s">
         <v>58</v>
       </c>
-      <c r="D32">
+      <c r="D32" t="s">
+        <v>39</v>
+      </c>
+      <c r="E32">
+        <v>83574</v>
+      </c>
+      <c r="F32">
         <v>121598</v>
       </c>
-      <c r="E32">
+      <c r="G32">
         <v>121365</v>
       </c>
-      <c r="F32">
+      <c r="H32">
         <v>234</v>
       </c>
     </row>
-    <row r="33" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C33" t="s">
         <v>59</v>
       </c>
-      <c r="D33">
+      <c r="D33" t="s">
+        <v>40</v>
+      </c>
+      <c r="E33">
+        <v>57918</v>
+      </c>
+      <c r="F33">
         <v>54475</v>
       </c>
-      <c r="E33">
+      <c r="G33">
         <v>47224</v>
       </c>
-      <c r="F33">
+      <c r="H33">
         <v>7251</v>
       </c>
     </row>
-    <row r="34" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C34" t="s">
         <v>60</v>
       </c>
-      <c r="D34">
+      <c r="D34" t="s">
+        <v>42</v>
+      </c>
+      <c r="E34">
+        <v>56276</v>
+      </c>
+      <c r="F34">
         <v>52672</v>
       </c>
-      <c r="E34">
+      <c r="G34">
         <v>48718</v>
       </c>
-      <c r="F34">
+      <c r="H34">
         <v>3954</v>
       </c>
     </row>
-    <row r="35" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C35" t="s">
         <v>61</v>
       </c>
-      <c r="D35">
+      <c r="D35" t="s">
+        <v>44</v>
+      </c>
+      <c r="E35">
+        <v>40411</v>
+      </c>
+      <c r="F35">
         <v>70704</v>
       </c>
-      <c r="E35">
+      <c r="G35">
         <v>68994</v>
       </c>
-      <c r="F35">
+      <c r="H35">
         <v>1710</v>
       </c>
     </row>
-    <row r="36" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C36" t="s">
         <v>62</v>
       </c>
-      <c r="D36">
+      <c r="D36" t="s">
+        <v>45</v>
+      </c>
+      <c r="E36">
+        <v>51843</v>
+      </c>
+      <c r="F36">
         <v>44828</v>
       </c>
-      <c r="E36">
+      <c r="G36">
         <v>40953</v>
       </c>
-      <c r="F36">
+      <c r="H36">
         <v>3875</v>
       </c>
     </row>
-    <row r="37" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C37" t="s">
         <v>63</v>
       </c>
-      <c r="D37">
+      <c r="D37" t="s">
+        <v>46</v>
+      </c>
+      <c r="E37">
+        <v>35387</v>
+      </c>
+      <c r="F37">
         <v>69903</v>
       </c>
-      <c r="E37">
+      <c r="G37">
         <v>68679</v>
       </c>
-      <c r="F37">
+      <c r="H37">
         <v>1224</v>
       </c>
     </row>
-    <row r="38" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C38" t="s">
         <v>64</v>
       </c>
-      <c r="D38">
+      <c r="D38" t="s">
+        <v>50</v>
+      </c>
+      <c r="E38">
+        <v>86943</v>
+      </c>
+      <c r="F38">
         <v>98386</v>
       </c>
-      <c r="E38">
+      <c r="G38">
         <v>96003</v>
       </c>
-      <c r="F38">
+      <c r="H38">
         <v>2383</v>
       </c>
     </row>
-    <row r="39" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C39" t="s">
         <v>65</v>
       </c>
-      <c r="D39">
+      <c r="D39" t="s">
+        <v>51</v>
+      </c>
+      <c r="E39">
+        <v>48434</v>
+      </c>
+      <c r="F39">
         <v>46058</v>
       </c>
-      <c r="E39">
+      <c r="G39">
         <v>44820</v>
       </c>
-      <c r="F39">
+      <c r="H39">
         <v>1239</v>
       </c>
     </row>
-    <row r="40" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C40" t="s">
         <v>66</v>
       </c>
-      <c r="D40">
+      <c r="D40" t="s">
+        <v>54</v>
+      </c>
+      <c r="E40">
+        <v>77358</v>
+      </c>
+      <c r="F40">
         <v>1545</v>
       </c>
-      <c r="E40">
+      <c r="G40">
         <v>1045</v>
       </c>
-      <c r="F40">
+      <c r="H40">
         <v>500</v>
       </c>
     </row>
-    <row r="41" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C41" t="s">
         <v>67</v>
       </c>
-      <c r="D41">
+      <c r="D41" t="s">
+        <v>55</v>
+      </c>
+      <c r="E41">
+        <v>110567</v>
+      </c>
+      <c r="F41">
         <v>32007</v>
       </c>
-      <c r="E41">
+      <c r="G41">
         <v>30111</v>
       </c>
-      <c r="F41">
+      <c r="H41">
         <v>1896</v>
       </c>
     </row>
-    <row r="42" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C42" t="s">
         <v>68</v>
       </c>
-      <c r="D42">
+      <c r="D42" t="s">
+        <v>61</v>
+      </c>
+      <c r="E42">
+        <v>70704</v>
+      </c>
+      <c r="F42">
         <v>77121</v>
       </c>
-      <c r="E42">
+      <c r="G42">
         <v>75898</v>
       </c>
-      <c r="F42">
+      <c r="H42">
         <v>1224</v>
       </c>
     </row>
-    <row r="43" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C43" t="s">
         <v>69</v>
       </c>
-      <c r="D43">
+      <c r="D43" t="s">
+        <v>63</v>
+      </c>
+      <c r="E43">
+        <v>69903</v>
+      </c>
+      <c r="F43">
         <v>42146</v>
       </c>
-      <c r="E43">
+      <c r="G43">
         <v>41220</v>
       </c>
-      <c r="F43">
+      <c r="H43">
         <v>926</v>
       </c>
     </row>
-    <row r="44" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C44" t="s">
         <v>70</v>
       </c>
-      <c r="D44">
+      <c r="D44" t="s">
+        <v>65</v>
+      </c>
+      <c r="E44">
+        <v>46058</v>
+      </c>
+      <c r="F44">
         <v>268601</v>
       </c>
-      <c r="E44">
+      <c r="G44">
         <v>261914</v>
       </c>
-      <c r="F44">
+      <c r="H44">
         <v>6687</v>
       </c>
     </row>
-    <row r="45" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C45" t="s">
         <v>71</v>
       </c>
-      <c r="D45">
+      <c r="D45" t="s">
+        <v>66</v>
+      </c>
+      <c r="E45">
+        <v>1545</v>
+      </c>
+      <c r="F45">
         <v>84904</v>
       </c>
-      <c r="E45">
+      <c r="G45">
         <v>82168</v>
       </c>
-      <c r="F45">
+      <c r="H45">
         <v>2736</v>
       </c>
     </row>
-    <row r="46" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C46" t="s">
         <v>73</v>
       </c>
-      <c r="D46">
+      <c r="D46" t="s">
+        <v>67</v>
+      </c>
+      <c r="E46">
+        <v>32007</v>
+      </c>
+      <c r="F46">
         <v>9615</v>
       </c>
-      <c r="E46">
+      <c r="G46">
         <v>9249</v>
       </c>
-      <c r="F46">
+      <c r="H46">
         <v>366</v>
       </c>
     </row>
-    <row r="47" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C47" t="s">
         <v>72</v>
       </c>
-      <c r="D47">
+      <c r="D47" t="s">
+        <v>69</v>
+      </c>
+      <c r="E47">
+        <v>42146</v>
+      </c>
+      <c r="F47">
         <v>42769</v>
       </c>
-      <c r="E47">
+      <c r="G47">
         <v>39598</v>
       </c>
-      <c r="F47">
+      <c r="H47">
         <v>3171</v>
       </c>
     </row>
-    <row r="48" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C48" t="s">
         <v>74</v>
       </c>
-      <c r="D48">
+      <c r="D48" t="s">
+        <v>73</v>
+      </c>
+      <c r="E48">
+        <v>9615</v>
+      </c>
+      <c r="F48">
         <v>71303</v>
       </c>
-      <c r="E48">
+      <c r="G48">
         <v>66582</v>
       </c>
-      <c r="F48">
+      <c r="H48">
         <v>4721</v>
       </c>
     </row>
-    <row r="49" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C49" t="s">
         <v>75</v>
       </c>
-      <c r="D49">
+      <c r="D49" t="s">
+        <v>72</v>
+      </c>
+      <c r="E49">
+        <v>42769</v>
+      </c>
+      <c r="F49">
         <v>24231</v>
       </c>
-      <c r="E49">
+      <c r="G49">
         <v>24087</v>
       </c>
-      <c r="F49">
+      <c r="H49">
         <v>145</v>
       </c>
     </row>
-    <row r="50" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C50" t="s">
         <v>76</v>
       </c>
-      <c r="D50">
+      <c r="D50" t="s">
+        <v>75</v>
+      </c>
+      <c r="E50">
+        <v>24231</v>
+      </c>
+      <c r="F50">
         <v>65503</v>
       </c>
-      <c r="E50">
+      <c r="G50">
         <v>54314</v>
       </c>
-      <c r="F50">
+      <c r="H50">
         <v>11190</v>
       </c>
     </row>
-    <row r="51" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C51" t="s">
         <v>77</v>
       </c>
-      <c r="D51">
+      <c r="D51" t="s">
+        <v>68</v>
+      </c>
+      <c r="E51">
+        <v>77121</v>
+      </c>
+      <c r="F51">
         <v>97818</v>
       </c>
-      <c r="E51">
+      <c r="G51">
         <v>97105</v>
       </c>
-      <c r="F51">
+      <c r="H51">
         <v>714</v>
       </c>
     </row>
-    <row r="52" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="3:8" x14ac:dyDescent="0.2">
       <c r="C52" t="s">
         <v>78</v>
       </c>
-      <c r="D52">
+      <c r="D52" t="s">
+        <v>78</v>
+      </c>
+      <c r="E52">
         <v>3515</v>
       </c>
     </row>
@@ -1495,5 +1824,8 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="61" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added to final file
added contingency table for each ecosystem
</commit_message>
<xml_diff>
--- a/SquareMileage.xlsx
+++ b/SquareMileage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/odalysbar/Documents/monmouthuni/MA321-FA20/MA321-Daneshgar/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{53D5D62A-D34A-494A-A753-4EF49B30539C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B0C5F61-CBE7-334D-BE92-6A42F90FF472}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14520" yWindow="0" windowWidth="14280" windowHeight="18000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="88">
   <si>
     <t>Continent</t>
   </si>
@@ -63,9 +63,6 @@
     <t>Land Sq. mi (mi^2)</t>
   </si>
   <si>
-    <t>Total Sq. mi (mi^2)</t>
-  </si>
-  <si>
     <t>Water Sq. mi (mi^2)</t>
   </si>
   <si>
@@ -286,6 +283,15 @@
   </si>
   <si>
     <t>stateSQM</t>
+  </si>
+  <si>
+    <t>state.In.Order</t>
+  </si>
+  <si>
+    <t>SM.IN.ORDER</t>
+  </si>
+  <si>
+    <t>Counts</t>
   </si>
 </sst>
 </file>
@@ -351,8 +357,22 @@
   <autoFilter ref="D1:F51" xr:uid="{F72EF95D-EC68-C742-80CD-2F052C045650}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{E474624B-F098-7749-8DDD-83082DC986CB}" name="U.S. States"/>
+    <tableColumn id="4" xr3:uid="{1B32EFEB-8C1D-B447-8971-9A9D0E7A4CF6}" name="Counts"/>
     <tableColumn id="3" xr3:uid="{DC7360F2-B0CA-F94C-937C-5C3A6028F94A}" name="stateSQM"/>
-    <tableColumn id="2" xr3:uid="{58FF40DC-05A5-CB44-B04E-A34E6EBCBDF5}" name="Total Sq. mi (mi^2)"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{C07FA604-9E08-D04C-B8C8-F3951444C56E}" name="Table5" displayName="Table5" ref="M1:N1048576" totalsRowShown="0">
+  <autoFilter ref="M1:N1048576" xr:uid="{AEAB1691-09D6-254A-9CA8-87AEF0FE0A27}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="M2:N1048576">
+    <sortCondition descending="1" ref="N1:N1048576"/>
+  </sortState>
+  <tableColumns count="2">
+    <tableColumn id="3" xr3:uid="{49E440F2-7A62-9A4B-AD9A-66AD1D96F3D9}" name="state.In.Order"/>
+    <tableColumn id="2" xr3:uid="{BA0A47EF-2000-0A46-8746-1A7A8EA435A8}" name="SM.IN.ORDER"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -624,19 +644,20 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L52"/>
+  <dimension ref="A1:N52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="140" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" zoomScale="140" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="11.6640625" customWidth="1"/>
-    <col min="5" max="5" width="18.1640625" customWidth="1"/>
+    <col min="4" max="5" width="11.6640625" customWidth="1"/>
+    <col min="6" max="6" width="18.1640625" customWidth="1"/>
+    <col min="13" max="14" width="18.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -647,48 +668,51 @@
         <v>9</v>
       </c>
       <c r="E1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F1" t="s">
-        <v>11</v>
+        <v>84</v>
       </c>
       <c r="G1" t="s">
         <v>10</v>
       </c>
       <c r="H1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" t="s">
         <v>12</v>
       </c>
-      <c r="I1" t="s">
-        <v>13</v>
-      </c>
       <c r="J1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+      <c r="M1" t="s">
+        <v>85</v>
+      </c>
+      <c r="N1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2">
         <v>9.5399999999999991</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>28</v>
       </c>
-      <c r="D2" t="s">
-        <v>29</v>
-      </c>
       <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
         <v>656424</v>
-      </c>
-      <c r="F2">
-        <v>52423</v>
       </c>
       <c r="G2">
         <v>50750</v>
@@ -697,36 +721,39 @@
         <v>1673</v>
       </c>
       <c r="I2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J2">
         <v>191308</v>
       </c>
       <c r="K2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L2">
         <v>161913</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M2" t="s">
+        <v>28</v>
+      </c>
+      <c r="N2">
+        <v>656424</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3">
         <v>6.8879999999999999</v>
       </c>
-      <c r="C3" t="s">
-        <v>29</v>
-      </c>
       <c r="D3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="F3">
         <v>52423</v>
-      </c>
-      <c r="F3">
-        <v>656424</v>
       </c>
       <c r="G3">
         <v>570374</v>
@@ -735,33 +762,36 @@
         <v>86051</v>
       </c>
       <c r="I3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J3">
         <v>292589</v>
       </c>
       <c r="K3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L3">
         <v>750576</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M3" t="s">
+        <v>69</v>
+      </c>
+      <c r="N3">
+        <v>268601</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4">
         <v>3.931</v>
       </c>
-      <c r="C4" t="s">
-        <v>30</v>
-      </c>
       <c r="D4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E4">
-        <v>114006</v>
+        <v>3</v>
       </c>
       <c r="F4">
         <v>114006</v>
@@ -773,36 +803,39 @@
         <v>364</v>
       </c>
       <c r="I4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J4">
         <v>299170</v>
       </c>
       <c r="K4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L4">
         <v>919331</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M4" t="s">
+        <v>31</v>
+      </c>
+      <c r="N4">
+        <v>163707</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5">
         <v>11.73</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>31</v>
       </c>
-      <c r="D5" t="s">
-        <v>32</v>
-      </c>
       <c r="E5">
+        <v>13</v>
+      </c>
+      <c r="F5">
         <v>163707</v>
-      </c>
-      <c r="F5">
-        <v>53182</v>
       </c>
       <c r="G5">
         <v>52075</v>
@@ -811,36 +844,39 @@
         <v>1107</v>
       </c>
       <c r="I5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J5">
         <v>5469</v>
       </c>
       <c r="K5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L5">
         <v>1873251</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M5" t="s">
+        <v>52</v>
+      </c>
+      <c r="N5">
+        <v>147046</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6">
         <v>17.21</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>32</v>
       </c>
-      <c r="D6" t="s">
-        <v>33</v>
-      </c>
       <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6">
         <v>104100</v>
-      </c>
-      <c r="F6">
-        <v>163707</v>
       </c>
       <c r="G6">
         <v>155973</v>
@@ -849,30 +885,33 @@
         <v>7734</v>
       </c>
       <c r="I6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+      <c r="M6" t="s">
+        <v>57</v>
+      </c>
+      <c r="N6">
+        <v>121598</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7">
         <v>2.97</v>
       </c>
-      <c r="C7" t="s">
-        <v>33</v>
-      </c>
       <c r="D7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E7">
+        <v>4</v>
+      </c>
+      <c r="F7">
         <v>59988</v>
-      </c>
-      <c r="F7">
-        <v>104100</v>
       </c>
       <c r="G7">
         <v>103730</v>
@@ -881,30 +920,33 @@
         <v>371</v>
       </c>
       <c r="I7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J7">
         <v>444100</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M7" t="s">
+        <v>29</v>
+      </c>
+      <c r="N7">
+        <v>114006</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
       <c r="B8">
         <v>3.2919999999999998</v>
       </c>
-      <c r="C8" t="s">
-        <v>34</v>
-      </c>
       <c r="D8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
         <v>6459</v>
-      </c>
-      <c r="F8">
-        <v>5544</v>
       </c>
       <c r="G8">
         <v>4845</v>
@@ -913,24 +955,27 @@
         <v>698</v>
       </c>
       <c r="I8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C9" t="s">
-        <v>35</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="M8" t="s">
+        <v>54</v>
+      </c>
+      <c r="N8">
+        <v>110567</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="D9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
         <v>36420</v>
-      </c>
-      <c r="F9">
-        <v>2489</v>
       </c>
       <c r="G9">
         <v>1955</v>
@@ -939,24 +984,27 @@
         <v>535</v>
       </c>
       <c r="I9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J9">
         <v>507900</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C10" t="s">
-        <v>36</v>
-      </c>
+      <c r="M9" t="s">
+        <v>32</v>
+      </c>
+      <c r="N9">
+        <v>104100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="D10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10">
         <v>82282</v>
-      </c>
-      <c r="F10">
-        <v>59988</v>
       </c>
       <c r="G10">
         <v>53997</v>
@@ -965,24 +1013,27 @@
         <v>5991</v>
       </c>
       <c r="I10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J10">
         <v>71992</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C11" t="s">
-        <v>37</v>
-      </c>
+      <c r="M10" t="s">
+        <v>63</v>
+      </c>
+      <c r="N10">
+        <v>98386</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="D11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
         <v>10555</v>
-      </c>
-      <c r="F11">
-        <v>59441</v>
       </c>
       <c r="G11">
         <v>57919</v>
@@ -991,24 +1042,27 @@
         <v>1522</v>
       </c>
       <c r="I11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C12" t="s">
-        <v>38</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="M11" t="s">
+        <v>76</v>
+      </c>
+      <c r="N11">
+        <v>97818</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="D12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
         <v>12407</v>
-      </c>
-      <c r="F12">
-        <v>6459</v>
       </c>
       <c r="G12">
         <v>6423</v>
@@ -1017,24 +1071,27 @@
         <v>36</v>
       </c>
       <c r="I12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C13" t="s">
-        <v>39</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="M12" t="s">
+        <v>48</v>
+      </c>
+      <c r="N12">
+        <v>96810</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="D13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E13">
+        <v>4</v>
+      </c>
+      <c r="F13">
         <v>96810</v>
-      </c>
-      <c r="F13">
-        <v>83574</v>
       </c>
       <c r="G13">
         <v>82751</v>
@@ -1043,24 +1100,27 @@
         <v>823</v>
       </c>
       <c r="I13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J13" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C14" t="s">
-        <v>40</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="M13" t="s">
+        <v>49</v>
+      </c>
+      <c r="N13">
+        <v>86943</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="D14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
         <v>69709</v>
-      </c>
-      <c r="F14">
-        <v>57918</v>
       </c>
       <c r="G14">
         <v>55593</v>
@@ -1068,19 +1128,22 @@
       <c r="H14">
         <v>2325</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C15" t="s">
-        <v>41</v>
-      </c>
+      <c r="M14" t="s">
+        <v>70</v>
+      </c>
+      <c r="N14">
+        <v>84904</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="D15" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
         <v>147046</v>
-      </c>
-      <c r="F15">
-        <v>36420</v>
       </c>
       <c r="G15">
         <v>35870</v>
@@ -1088,19 +1151,22 @@
       <c r="H15">
         <v>550</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C16" t="s">
-        <v>42</v>
-      </c>
+      <c r="M15" t="s">
+        <v>38</v>
+      </c>
+      <c r="N15">
+        <v>83574</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="D16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
         <v>52672</v>
-      </c>
-      <c r="F16">
-        <v>56276</v>
       </c>
       <c r="G16">
         <v>55875</v>
@@ -1108,19 +1174,22 @@
       <c r="H16">
         <v>401</v>
       </c>
-    </row>
-    <row r="17" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C17" t="s">
-        <v>43</v>
-      </c>
+      <c r="M16" t="s">
+        <v>42</v>
+      </c>
+      <c r="N16">
+        <v>82282</v>
+      </c>
+    </row>
+    <row r="17" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
         <v>9351</v>
-      </c>
-      <c r="F17">
-        <v>82282</v>
       </c>
       <c r="G17">
         <v>81823</v>
@@ -1128,19 +1197,22 @@
       <c r="H17">
         <v>459</v>
       </c>
-    </row>
-    <row r="18" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C18" t="s">
-        <v>44</v>
-      </c>
+      <c r="M17" t="s">
+        <v>53</v>
+      </c>
+      <c r="N17">
+        <v>77358</v>
+      </c>
+    </row>
+    <row r="18" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E18">
+        <v>2</v>
+      </c>
+      <c r="F18">
         <v>8722</v>
-      </c>
-      <c r="F18">
-        <v>40411</v>
       </c>
       <c r="G18">
         <v>39732</v>
@@ -1148,19 +1220,22 @@
       <c r="H18">
         <v>679</v>
       </c>
-    </row>
-    <row r="19" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C19" t="s">
-        <v>45</v>
-      </c>
+      <c r="M18" t="s">
+        <v>67</v>
+      </c>
+      <c r="N18">
+        <v>77121</v>
+      </c>
+    </row>
+    <row r="19" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
         <v>121598</v>
-      </c>
-      <c r="F19">
-        <v>51843</v>
       </c>
       <c r="G19">
         <v>43566</v>
@@ -1168,19 +1243,22 @@
       <c r="H19">
         <v>8277</v>
       </c>
-    </row>
-    <row r="20" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C20" t="s">
-        <v>46</v>
-      </c>
+      <c r="M19" t="s">
+        <v>73</v>
+      </c>
+      <c r="N19">
+        <v>71303</v>
+      </c>
+    </row>
+    <row r="20" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
         <v>54475</v>
-      </c>
-      <c r="F20">
-        <v>35387</v>
       </c>
       <c r="G20">
         <v>30865</v>
@@ -1188,19 +1266,22 @@
       <c r="H20">
         <v>4523</v>
       </c>
-    </row>
-    <row r="21" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C21" t="s">
-        <v>47</v>
-      </c>
+      <c r="M20" t="s">
+        <v>60</v>
+      </c>
+      <c r="N20">
+        <v>70704</v>
+      </c>
+    </row>
+    <row r="21" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
         <v>44828</v>
-      </c>
-      <c r="F21">
-        <v>12407</v>
       </c>
       <c r="G21">
         <v>9775</v>
@@ -1208,19 +1289,22 @@
       <c r="H21">
         <v>2633</v>
       </c>
-    </row>
-    <row r="22" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C22" t="s">
-        <v>48</v>
-      </c>
+      <c r="M21" t="s">
+        <v>62</v>
+      </c>
+      <c r="N21">
+        <v>69903</v>
+      </c>
+    </row>
+    <row r="22" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D22" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E22">
+        <v>4</v>
+      </c>
+      <c r="F22">
         <v>98386</v>
-      </c>
-      <c r="F22">
-        <v>10555</v>
       </c>
       <c r="G22">
         <v>7838</v>
@@ -1228,19 +1312,22 @@
       <c r="H22">
         <v>2717</v>
       </c>
-    </row>
-    <row r="23" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C23" t="s">
-        <v>49</v>
-      </c>
+      <c r="M22" t="s">
+        <v>51</v>
+      </c>
+      <c r="N22">
+        <v>69709</v>
+      </c>
+    </row>
+    <row r="23" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E23">
+        <v>3</v>
+      </c>
+      <c r="F23">
         <v>268601</v>
-      </c>
-      <c r="F23">
-        <v>96810</v>
       </c>
       <c r="G23">
         <v>56809</v>
@@ -1248,19 +1335,22 @@
       <c r="H23">
         <v>40001</v>
       </c>
-    </row>
-    <row r="24" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C24" t="s">
-        <v>50</v>
-      </c>
+      <c r="M23" t="s">
+        <v>75</v>
+      </c>
+      <c r="N23">
+        <v>65503</v>
+      </c>
+    </row>
+    <row r="24" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D24" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
         <v>84904</v>
-      </c>
-      <c r="F24">
-        <v>86943</v>
       </c>
       <c r="G24">
         <v>79617</v>
@@ -1268,19 +1358,22 @@
       <c r="H24">
         <v>7326</v>
       </c>
-    </row>
-    <row r="25" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C25" t="s">
-        <v>51</v>
-      </c>
+      <c r="M24" t="s">
+        <v>35</v>
+      </c>
+      <c r="N24">
+        <v>59988</v>
+      </c>
+    </row>
+    <row r="25" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E25">
+        <v>3</v>
+      </c>
+      <c r="F25">
         <v>71303</v>
-      </c>
-      <c r="F25">
-        <v>48434</v>
       </c>
       <c r="G25">
         <v>46914</v>
@@ -1288,19 +1381,22 @@
       <c r="H25">
         <v>1520</v>
       </c>
-    </row>
-    <row r="26" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C26" t="s">
-        <v>52</v>
-      </c>
+      <c r="M25" t="s">
+        <v>36</v>
+      </c>
+      <c r="N25">
+        <v>59441</v>
+      </c>
+    </row>
+    <row r="26" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
         <v>65503</v>
-      </c>
-      <c r="F26">
-        <v>69709</v>
       </c>
       <c r="G26">
         <v>68898</v>
@@ -1308,19 +1404,22 @@
       <c r="H26">
         <v>811</v>
       </c>
-    </row>
-    <row r="27" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C27" t="s">
-        <v>53</v>
-      </c>
+      <c r="M26" t="s">
+        <v>39</v>
+      </c>
+      <c r="N26">
+        <v>57918</v>
+      </c>
+    </row>
+    <row r="27" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D27" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E27">
+        <v>2</v>
+      </c>
+      <c r="F27">
         <v>97818</v>
-      </c>
-      <c r="F27">
-        <v>147046</v>
       </c>
       <c r="G27">
         <v>145556</v>
@@ -1328,19 +1427,22 @@
       <c r="H27">
         <v>1490</v>
       </c>
-    </row>
-    <row r="28" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C28" t="s">
-        <v>54</v>
-      </c>
+      <c r="M27" t="s">
+        <v>41</v>
+      </c>
+      <c r="N27">
+        <v>56276</v>
+      </c>
+    </row>
+    <row r="28" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
         <v>53182</v>
-      </c>
-      <c r="F28">
-        <v>77358</v>
       </c>
       <c r="G28">
         <v>76878</v>
@@ -1348,19 +1450,22 @@
       <c r="H28">
         <v>481</v>
       </c>
-    </row>
-    <row r="29" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C29" t="s">
-        <v>55</v>
-      </c>
+      <c r="M28" t="s">
+        <v>58</v>
+      </c>
+      <c r="N28">
+        <v>54475</v>
+      </c>
+    </row>
+    <row r="29" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
         <v>5544</v>
-      </c>
-      <c r="F29">
-        <v>110567</v>
       </c>
       <c r="G29">
         <v>109806</v>
@@ -1368,19 +1473,22 @@
       <c r="H29">
         <v>761</v>
       </c>
-    </row>
-    <row r="30" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C30" t="s">
-        <v>56</v>
-      </c>
+      <c r="M29" t="s">
+        <v>30</v>
+      </c>
+      <c r="N29">
+        <v>53182</v>
+      </c>
+    </row>
+    <row r="30" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
         <v>2489</v>
-      </c>
-      <c r="F30">
-        <v>9351</v>
       </c>
       <c r="G30">
         <v>8969</v>
@@ -1388,19 +1496,22 @@
       <c r="H30">
         <v>382</v>
       </c>
-    </row>
-    <row r="31" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C31" t="s">
-        <v>57</v>
-      </c>
+      <c r="M30" t="s">
+        <v>59</v>
+      </c>
+      <c r="N30">
+        <v>52672</v>
+      </c>
+    </row>
+    <row r="31" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D31" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
         <v>59441</v>
-      </c>
-      <c r="F31">
-        <v>8722</v>
       </c>
       <c r="G31">
         <v>7419</v>
@@ -1408,19 +1519,22 @@
       <c r="H31">
         <v>1303</v>
       </c>
-    </row>
-    <row r="32" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C32" t="s">
-        <v>58</v>
-      </c>
+      <c r="M31" t="s">
+        <v>27</v>
+      </c>
+      <c r="N31">
+        <v>52423</v>
+      </c>
+    </row>
+    <row r="32" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D32" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
         <v>83574</v>
-      </c>
-      <c r="F32">
-        <v>121598</v>
       </c>
       <c r="G32">
         <v>121365</v>
@@ -1428,19 +1542,22 @@
       <c r="H32">
         <v>234</v>
       </c>
-    </row>
-    <row r="33" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C33" t="s">
-        <v>59</v>
-      </c>
+      <c r="M32" t="s">
+        <v>44</v>
+      </c>
+      <c r="N32">
+        <v>51843</v>
+      </c>
+    </row>
+    <row r="33" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D33" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
         <v>57918</v>
-      </c>
-      <c r="F33">
-        <v>54475</v>
       </c>
       <c r="G33">
         <v>47224</v>
@@ -1448,19 +1565,22 @@
       <c r="H33">
         <v>7251</v>
       </c>
-    </row>
-    <row r="34" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C34" t="s">
-        <v>60</v>
-      </c>
+      <c r="M33" t="s">
+        <v>50</v>
+      </c>
+      <c r="N33">
+        <v>48434</v>
+      </c>
+    </row>
+    <row r="34" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D34" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
         <v>56276</v>
-      </c>
-      <c r="F34">
-        <v>52672</v>
       </c>
       <c r="G34">
         <v>48718</v>
@@ -1468,19 +1588,22 @@
       <c r="H34">
         <v>3954</v>
       </c>
-    </row>
-    <row r="35" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C35" t="s">
-        <v>61</v>
-      </c>
+      <c r="M34" t="s">
+        <v>64</v>
+      </c>
+      <c r="N34">
+        <v>46058</v>
+      </c>
+    </row>
+    <row r="35" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D35" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
         <v>40411</v>
-      </c>
-      <c r="F35">
-        <v>70704</v>
       </c>
       <c r="G35">
         <v>68994</v>
@@ -1488,19 +1611,22 @@
       <c r="H35">
         <v>1710</v>
       </c>
-    </row>
-    <row r="36" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C36" t="s">
-        <v>62</v>
-      </c>
+      <c r="M35" t="s">
+        <v>61</v>
+      </c>
+      <c r="N35">
+        <v>44828</v>
+      </c>
+    </row>
+    <row r="36" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D36" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36">
         <v>51843</v>
-      </c>
-      <c r="F36">
-        <v>44828</v>
       </c>
       <c r="G36">
         <v>40953</v>
@@ -1508,19 +1634,22 @@
       <c r="H36">
         <v>3875</v>
       </c>
-    </row>
-    <row r="37" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C37" t="s">
-        <v>63</v>
-      </c>
+      <c r="M36" t="s">
+        <v>71</v>
+      </c>
+      <c r="N36">
+        <v>42769</v>
+      </c>
+    </row>
+    <row r="37" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D37" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37">
         <v>35387</v>
-      </c>
-      <c r="F37">
-        <v>69903</v>
       </c>
       <c r="G37">
         <v>68679</v>
@@ -1528,19 +1657,22 @@
       <c r="H37">
         <v>1224</v>
       </c>
-    </row>
-    <row r="38" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C38" t="s">
-        <v>64</v>
-      </c>
+      <c r="M37" t="s">
+        <v>68</v>
+      </c>
+      <c r="N37">
+        <v>42146</v>
+      </c>
+    </row>
+    <row r="38" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D38" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38">
         <v>86943</v>
-      </c>
-      <c r="F38">
-        <v>98386</v>
       </c>
       <c r="G38">
         <v>96003</v>
@@ -1548,19 +1680,22 @@
       <c r="H38">
         <v>2383</v>
       </c>
-    </row>
-    <row r="39" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C39" t="s">
-        <v>65</v>
-      </c>
+      <c r="M38" t="s">
+        <v>43</v>
+      </c>
+      <c r="N38">
+        <v>40411</v>
+      </c>
+    </row>
+    <row r="39" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D39" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
         <v>48434</v>
-      </c>
-      <c r="F39">
-        <v>46058</v>
       </c>
       <c r="G39">
         <v>44820</v>
@@ -1568,19 +1703,22 @@
       <c r="H39">
         <v>1239</v>
       </c>
-    </row>
-    <row r="40" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C40" t="s">
-        <v>66</v>
-      </c>
+      <c r="M39" t="s">
+        <v>40</v>
+      </c>
+      <c r="N39">
+        <v>36420</v>
+      </c>
+    </row>
+    <row r="40" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D40" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40">
         <v>77358</v>
-      </c>
-      <c r="F40">
-        <v>1545</v>
       </c>
       <c r="G40">
         <v>1045</v>
@@ -1588,19 +1726,22 @@
       <c r="H40">
         <v>500</v>
       </c>
-    </row>
-    <row r="41" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C41" t="s">
-        <v>67</v>
-      </c>
+      <c r="M40" t="s">
+        <v>45</v>
+      </c>
+      <c r="N40">
+        <v>35387</v>
+      </c>
+    </row>
+    <row r="41" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D41" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41">
         <v>110567</v>
-      </c>
-      <c r="F41">
-        <v>32007</v>
       </c>
       <c r="G41">
         <v>30111</v>
@@ -1608,19 +1749,22 @@
       <c r="H41">
         <v>1896</v>
       </c>
-    </row>
-    <row r="42" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C42" t="s">
-        <v>68</v>
-      </c>
+      <c r="M41" t="s">
+        <v>66</v>
+      </c>
+      <c r="N41">
+        <v>32007</v>
+      </c>
+    </row>
+    <row r="42" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D42" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42">
         <v>70704</v>
-      </c>
-      <c r="F42">
-        <v>77121</v>
       </c>
       <c r="G42">
         <v>75898</v>
@@ -1628,19 +1772,22 @@
       <c r="H42">
         <v>1224</v>
       </c>
-    </row>
-    <row r="43" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C43" t="s">
-        <v>69</v>
-      </c>
+      <c r="M42" t="s">
+        <v>74</v>
+      </c>
+      <c r="N42">
+        <v>24231</v>
+      </c>
+    </row>
+    <row r="43" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D43" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43">
         <v>69903</v>
-      </c>
-      <c r="F43">
-        <v>42146</v>
       </c>
       <c r="G43">
         <v>41220</v>
@@ -1648,19 +1795,22 @@
       <c r="H43">
         <v>926</v>
       </c>
-    </row>
-    <row r="44" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C44" t="s">
-        <v>70</v>
-      </c>
+      <c r="M43" t="s">
+        <v>46</v>
+      </c>
+      <c r="N43">
+        <v>12407</v>
+      </c>
+    </row>
+    <row r="44" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D44" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44">
         <v>46058</v>
-      </c>
-      <c r="F44">
-        <v>268601</v>
       </c>
       <c r="G44">
         <v>261914</v>
@@ -1668,19 +1818,22 @@
       <c r="H44">
         <v>6687</v>
       </c>
-    </row>
-    <row r="45" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C45" t="s">
-        <v>71</v>
-      </c>
+      <c r="M44" t="s">
+        <v>47</v>
+      </c>
+      <c r="N44">
+        <v>10555</v>
+      </c>
+    </row>
+    <row r="45" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D45" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45">
         <v>1545</v>
-      </c>
-      <c r="F45">
-        <v>84904</v>
       </c>
       <c r="G45">
         <v>82168</v>
@@ -1688,19 +1841,22 @@
       <c r="H45">
         <v>2736</v>
       </c>
-    </row>
-    <row r="46" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C46" t="s">
-        <v>73</v>
-      </c>
+      <c r="M45" t="s">
+        <v>72</v>
+      </c>
+      <c r="N45">
+        <v>9615</v>
+      </c>
+    </row>
+    <row r="46" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D46" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46">
         <v>32007</v>
-      </c>
-      <c r="F46">
-        <v>9615</v>
       </c>
       <c r="G46">
         <v>9249</v>
@@ -1708,19 +1864,22 @@
       <c r="H46">
         <v>366</v>
       </c>
-    </row>
-    <row r="47" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C47" t="s">
-        <v>72</v>
-      </c>
+      <c r="M46" t="s">
+        <v>55</v>
+      </c>
+      <c r="N46">
+        <v>9351</v>
+      </c>
+    </row>
+    <row r="47" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D47" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="F47">
         <v>42146</v>
-      </c>
-      <c r="F47">
-        <v>42769</v>
       </c>
       <c r="G47">
         <v>39598</v>
@@ -1728,19 +1887,22 @@
       <c r="H47">
         <v>3171</v>
       </c>
-    </row>
-    <row r="48" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C48" t="s">
-        <v>74</v>
-      </c>
+      <c r="M47" t="s">
+        <v>56</v>
+      </c>
+      <c r="N47">
+        <v>8722</v>
+      </c>
+    </row>
+    <row r="48" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D48" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E48">
+        <v>0</v>
+      </c>
+      <c r="F48">
         <v>9615</v>
-      </c>
-      <c r="F48">
-        <v>71303</v>
       </c>
       <c r="G48">
         <v>66582</v>
@@ -1748,19 +1910,22 @@
       <c r="H48">
         <v>4721</v>
       </c>
-    </row>
-    <row r="49" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C49" t="s">
-        <v>75</v>
-      </c>
+      <c r="M48" t="s">
+        <v>37</v>
+      </c>
+      <c r="N48">
+        <v>6459</v>
+      </c>
+    </row>
+    <row r="49" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D49" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E49">
+        <v>0</v>
+      </c>
+      <c r="F49">
         <v>42769</v>
-      </c>
-      <c r="F49">
-        <v>24231</v>
       </c>
       <c r="G49">
         <v>24087</v>
@@ -1768,19 +1933,22 @@
       <c r="H49">
         <v>145</v>
       </c>
-    </row>
-    <row r="50" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C50" t="s">
-        <v>76</v>
-      </c>
+      <c r="M49" t="s">
+        <v>33</v>
+      </c>
+      <c r="N49">
+        <v>5544</v>
+      </c>
+    </row>
+    <row r="50" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D50" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E50">
+        <v>0</v>
+      </c>
+      <c r="F50">
         <v>24231</v>
-      </c>
-      <c r="F50">
-        <v>65503</v>
       </c>
       <c r="G50">
         <v>54314</v>
@@ -1788,19 +1956,22 @@
       <c r="H50">
         <v>11190</v>
       </c>
-    </row>
-    <row r="51" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C51" t="s">
-        <v>77</v>
-      </c>
+      <c r="M50" t="s">
+        <v>34</v>
+      </c>
+      <c r="N50">
+        <v>2489</v>
+      </c>
+    </row>
+    <row r="51" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D51" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E51">
+        <v>0</v>
+      </c>
+      <c r="F51">
         <v>77121</v>
-      </c>
-      <c r="F51">
-        <v>97818</v>
       </c>
       <c r="G51">
         <v>97105</v>
@@ -1808,15 +1979,18 @@
       <c r="H51">
         <v>714</v>
       </c>
-    </row>
-    <row r="52" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C52" t="s">
-        <v>78</v>
-      </c>
+      <c r="M51" t="s">
+        <v>65</v>
+      </c>
+      <c r="N51">
+        <v>1545</v>
+      </c>
+    </row>
+    <row r="52" spans="4:14" x14ac:dyDescent="0.2">
       <c r="D52" t="s">
-        <v>78</v>
-      </c>
-      <c r="E52">
+        <v>77</v>
+      </c>
+      <c r="F52">
         <v>3515</v>
       </c>
     </row>
@@ -1824,8 +1998,9 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="61" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
-  <tableParts count="1">
+  <tableParts count="2">
     <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>